<commit_message>
Word scoring method changed and added some explanation
</commit_message>
<xml_diff>
--- a/ssnmf_words.xlsx
+++ b/ssnmf_words.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="211">
   <si>
     <t>universalism - word</t>
   </si>
@@ -86,277 +86,544 @@
     <t>group</t>
   </si>
   <si>
+    <t>intern</t>
+  </si>
+  <si>
+    <t>peopl</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>develop</t>
+  </si>
+  <si>
+    <t>govern</t>
+  </si>
+  <si>
+    <t>econom</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>take</t>
+  </si>
+  <si>
+    <t>BENEVOLENCE</t>
+  </si>
+  <si>
+    <t>natur</t>
+  </si>
+  <si>
+    <t>theori</t>
+  </si>
+  <si>
+    <t>seem</t>
+  </si>
+  <si>
+    <t>need</t>
+  </si>
+  <si>
+    <t>sometim</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>exampl</t>
+  </si>
+  <si>
+    <t>mani</t>
+  </si>
+  <si>
+    <t>CONFORMITY</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>thu</t>
+  </si>
+  <si>
+    <t>great</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
+  <si>
+    <t>sourc</t>
+  </si>
+  <si>
+    <t>uncodifi</t>
+  </si>
+  <si>
+    <t>still</t>
+  </si>
+  <si>
+    <t>refer</t>
+  </si>
+  <si>
+    <t>TRADITION</t>
+  </si>
+  <si>
+    <t>particularli</t>
+  </si>
+  <si>
+    <t>thing</t>
+  </si>
+  <si>
+    <t>sinc</t>
+  </si>
+  <si>
+    <t>preciou</t>
+  </si>
+  <si>
+    <t>gener</t>
+  </si>
+  <si>
+    <t>steal</t>
+  </si>
+  <si>
+    <t>generos</t>
+  </si>
+  <si>
+    <t>examin</t>
+  </si>
+  <si>
+    <t>temper</t>
+  </si>
+  <si>
+    <t>SECURITY</t>
+  </si>
+  <si>
+    <t>evid</t>
+  </si>
+  <si>
+    <t>fals</t>
+  </si>
+  <si>
+    <t>someth</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>sever</t>
+  </si>
+  <si>
+    <t>indic</t>
+  </si>
+  <si>
+    <t>dynam</t>
+  </si>
+  <si>
+    <t>techniqu</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>articl</t>
+  </si>
+  <si>
+    <t>leadership</t>
+  </si>
+  <si>
+    <t>idea</t>
+  </si>
+  <si>
+    <t>toxic</t>
+  </si>
+  <si>
+    <t>environ</t>
+  </si>
+  <si>
+    <t>belong</t>
+  </si>
+  <si>
+    <t>law</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>ACHIEVEMENT</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>merchant</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>known</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>HEDONISM</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>see</t>
+  </si>
+  <si>
+    <t>reaction</t>
+  </si>
+  <si>
+    <t>studi</t>
+  </si>
+  <si>
+    <t>repres</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>think</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>simpli</t>
+  </si>
+  <si>
+    <t>STIMULATION</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>fun</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>suffer</t>
+  </si>
+  <si>
+    <t>miyazaki</t>
+  </si>
+  <si>
+    <t>psycholog</t>
+  </si>
+  <si>
+    <t>declin</t>
+  </si>
+  <si>
+    <t>remov</t>
+  </si>
+  <si>
+    <t>fare</t>
+  </si>
+  <si>
+    <t>SELF-DIRECTION</t>
+  </si>
+  <si>
+    <t>made</t>
+  </si>
+  <si>
+    <t>variou</t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>resent</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>reminisc</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
     <t>state</t>
   </si>
   <si>
-    <t>peopl</t>
-  </si>
-  <si>
     <t>human</t>
   </si>
   <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>intern</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>form</t>
-  </si>
-  <si>
-    <t>world</t>
-  </si>
-  <si>
-    <t>refer</t>
-  </si>
-  <si>
-    <t>BENEVOLENCE</t>
-  </si>
-  <si>
     <t>one</t>
   </si>
   <si>
-    <t>sometim</t>
-  </si>
-  <si>
-    <t>natur</t>
-  </si>
-  <si>
-    <t>theori</t>
+    <t>upon</t>
+  </si>
+  <si>
+    <t>automat</t>
   </si>
   <si>
     <t>view</t>
   </si>
   <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>thought</t>
-  </si>
-  <si>
-    <t>need</t>
-  </si>
-  <si>
-    <t>upon</t>
-  </si>
-  <si>
-    <t>seem</t>
-  </si>
-  <si>
-    <t>CONFORMITY</t>
-  </si>
-  <si>
-    <t>show</t>
-  </si>
-  <si>
-    <t>use</t>
-  </si>
-  <si>
-    <t>thu</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>sourc</t>
-  </si>
-  <si>
-    <t>great</t>
-  </si>
-  <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>TRADITION</t>
-  </si>
-  <si>
-    <t>particularli</t>
+    <t>realiti</t>
+  </si>
+  <si>
+    <t>translat</t>
+  </si>
+  <si>
+    <t>introduc</t>
+  </si>
+  <si>
+    <t>uneduc</t>
+  </si>
+  <si>
+    <t>attempt</t>
+  </si>
+  <si>
+    <t>precondit</t>
+  </si>
+  <si>
+    <t>incom</t>
+  </si>
+  <si>
+    <t>paint</t>
+  </si>
+  <si>
+    <t>mose</t>
+  </si>
+  <si>
+    <t>antiquitatem</t>
   </si>
   <si>
     <t>passion</t>
   </si>
   <si>
-    <t>sinc</t>
-  </si>
-  <si>
-    <t>thing</t>
-  </si>
-  <si>
-    <t>antiquitatem</t>
-  </si>
-  <si>
-    <t>law</t>
-  </si>
-  <si>
-    <t>preciou</t>
-  </si>
-  <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>help</t>
+    <t>simon</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
   <si>
     <t>three</t>
   </si>
   <si>
-    <t>SECURITY</t>
+    <t>twice</t>
+  </si>
+  <si>
+    <t>regal</t>
+  </si>
+  <si>
+    <t>illustr</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>thousand</t>
+  </si>
+  <si>
+    <t>pollut</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
+    <t>relat</t>
+  </si>
+  <si>
+    <t>poorer</t>
+  </si>
+  <si>
+    <t>jablonski</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>motiv</t>
+  </si>
+  <si>
+    <t>tribe</t>
+  </si>
+  <si>
+    <t>practic</t>
+  </si>
+  <si>
+    <t>within</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>western</t>
+  </si>
+  <si>
+    <t>would</t>
+  </si>
+  <si>
+    <t>theolog</t>
+  </si>
+  <si>
+    <t>shut</t>
+  </si>
+  <si>
+    <t>act</t>
+  </si>
+  <si>
+    <t>typic</t>
+  </si>
+  <si>
+    <t>pleasur</t>
+  </si>
+  <si>
+    <t>matt</t>
+  </si>
+  <si>
+    <t>benedek</t>
+  </si>
+  <si>
+    <t>romantic</t>
+  </si>
+  <si>
+    <t>liberti</t>
+  </si>
+  <si>
+    <t>domin</t>
+  </si>
+  <si>
+    <t>olivero</t>
+  </si>
+  <si>
+    <t>ratifi</t>
+  </si>
+  <si>
+    <t>london</t>
+  </si>
+  <si>
+    <t>tendenc</t>
+  </si>
+  <si>
+    <t>parti</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>portal</t>
+  </si>
+  <si>
+    <t>renew</t>
+  </si>
+  <si>
+    <t>mythomania</t>
+  </si>
+  <si>
+    <t>definit</t>
+  </si>
+  <si>
+    <t>collectivist</t>
+  </si>
+  <si>
+    <t>voltag</t>
+  </si>
+  <si>
+    <t>rewritten</t>
+  </si>
+  <si>
+    <t>undesir</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>valuabl</t>
+  </si>
+  <si>
+    <t>sauda</t>
   </si>
   <si>
     <t>signific</t>
   </si>
   <si>
-    <t>relat</t>
-  </si>
-  <si>
-    <t>land</t>
-  </si>
-  <si>
-    <t>play</t>
-  </si>
-  <si>
-    <t>evid</t>
-  </si>
-  <si>
-    <t>pollut</t>
-  </si>
-  <si>
-    <t>someth</t>
-  </si>
-  <si>
-    <t>fals</t>
-  </si>
-  <si>
-    <t>POWER</t>
-  </si>
-  <si>
-    <t>leadership</t>
-  </si>
-  <si>
-    <t>articl</t>
-  </si>
-  <si>
-    <t>may</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>idea</t>
-  </si>
-  <si>
-    <t>least</t>
-  </si>
-  <si>
-    <t>compos</t>
-  </si>
-  <si>
-    <t>ACHIEVEMENT</t>
-  </si>
-  <si>
-    <t>social</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>work</t>
-  </si>
-  <si>
-    <t>loan</t>
-  </si>
-  <si>
-    <t>HEDONISM</t>
-  </si>
-  <si>
-    <t>see</t>
-  </si>
-  <si>
-    <t>studi</t>
-  </si>
-  <si>
-    <t>psycholog</t>
-  </si>
-  <si>
-    <t>shock</t>
-  </si>
-  <si>
-    <t>self</t>
-  </si>
-  <si>
-    <t>repres</t>
+    <t>pesticid</t>
+  </si>
+  <si>
+    <t>mechan</t>
+  </si>
+  <si>
+    <t>reopen</t>
+  </si>
+  <si>
+    <t>union</t>
   </si>
   <si>
     <t>seri</t>
   </si>
   <si>
-    <t>STIMULATION</t>
-  </si>
-  <si>
-    <t>reason</t>
-  </si>
-  <si>
-    <t>risk</t>
-  </si>
-  <si>
-    <t>indic</t>
-  </si>
-  <si>
-    <t>fun</t>
+    <t>surpris</t>
   </si>
   <si>
     <t>exo</t>
   </si>
   <si>
-    <t>miyazaki</t>
-  </si>
-  <si>
-    <t>declin</t>
-  </si>
-  <si>
-    <t>suffer</t>
-  </si>
-  <si>
-    <t>SELF-DIRECTION</t>
-  </si>
-  <si>
-    <t>well</t>
-  </si>
-  <si>
-    <t>gener</t>
-  </si>
-  <si>
-    <t>take</t>
-  </si>
-  <si>
-    <t>known</t>
-  </si>
-  <si>
-    <t>made</t>
-  </si>
-  <si>
-    <t>resourc</t>
-  </si>
-  <si>
-    <t>benedek</t>
-  </si>
-  <si>
-    <t>romantic</t>
-  </si>
-  <si>
-    <t>liberti</t>
+    <t>ongo</t>
+  </si>
+  <si>
+    <t>mainli</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>reliabl</t>
+  </si>
+  <si>
+    <t>opportun</t>
   </si>
   <si>
     <t>zzz</t>
@@ -826,7 +1093,7 @@
         <v>62.966</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>77.557</v>
@@ -838,7 +1105,7 @@
         <v>38.482</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <v>17.296</v>
@@ -856,19 +1123,19 @@
         <v>44.738</v>
       </c>
       <c r="P2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q2">
         <v>51.584</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S2">
         <v>41.783</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="U2">
         <v>49.243</v>
@@ -882,61 +1149,61 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>38.667</v>
+        <v>0.491</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3">
-        <v>43.643</v>
+        <v>1.088</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3">
-        <v>66.63500000000001</v>
+        <v>1.835</v>
       </c>
       <c r="H3" t="s">
         <v>53</v>
       </c>
       <c r="I3">
-        <v>21.811</v>
+        <v>0.716</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="K3">
-        <v>10.678</v>
+        <v>0.229</v>
       </c>
       <c r="L3" t="s">
         <v>73</v>
       </c>
       <c r="M3">
-        <v>28.442</v>
+        <v>0.493</v>
       </c>
       <c r="N3" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="O3">
-        <v>39.456</v>
+        <v>0.922</v>
       </c>
       <c r="P3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Q3">
-        <v>79.625</v>
+        <v>1.254</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="S3">
-        <v>24.053</v>
+        <v>0.595</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="U3">
-        <v>44.256</v>
+        <v>1.147</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -947,61 +1214,61 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>28.641</v>
+        <v>0.301</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
       <c r="E4">
-        <v>43.034</v>
+        <v>1.079</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4">
-        <v>65.607</v>
+        <v>1.78</v>
       </c>
       <c r="H4" t="s">
         <v>54</v>
       </c>
       <c r="I4">
-        <v>20.097</v>
+        <v>0.634</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="K4">
-        <v>9.698</v>
+        <v>0.223</v>
       </c>
       <c r="L4" t="s">
         <v>74</v>
       </c>
       <c r="M4">
-        <v>27.959</v>
+        <v>0.443</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="O4">
-        <v>37.12</v>
+        <v>0.883</v>
       </c>
       <c r="P4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q4">
-        <v>64.634</v>
+        <v>1.036</v>
       </c>
       <c r="R4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="S4">
-        <v>23.527</v>
+        <v>0.526</v>
       </c>
       <c r="T4" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="U4">
-        <v>35.769</v>
+        <v>1.119</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1012,61 +1279,61 @@
         <v>23</v>
       </c>
       <c r="C5">
-        <v>27.913</v>
+        <v>0.296</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
       </c>
       <c r="E5">
-        <v>42.042</v>
+        <v>1.046</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5">
-        <v>55.297</v>
+        <v>1.568</v>
       </c>
       <c r="H5" t="s">
         <v>55</v>
       </c>
       <c r="I5">
-        <v>19.348</v>
+        <v>0.618</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5">
-        <v>9.272</v>
+        <v>0.216</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M5">
-        <v>27.621</v>
+        <v>0.37</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="O5">
-        <v>35.759</v>
+        <v>0.78</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="Q5">
-        <v>64.292</v>
+        <v>1.015</v>
       </c>
       <c r="R5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="S5">
-        <v>22.968</v>
+        <v>0.454</v>
       </c>
       <c r="T5" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="U5">
-        <v>33.186</v>
+        <v>1.086</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1077,61 +1344,61 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>25.094</v>
+        <v>0.283</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
       </c>
       <c r="E6">
-        <v>41.727</v>
+        <v>1.015</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6">
-        <v>54.415</v>
+        <v>1.512</v>
       </c>
       <c r="H6" t="s">
         <v>56</v>
       </c>
       <c r="I6">
-        <v>19.208</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="K6">
-        <v>9.188000000000001</v>
+        <v>0.205</v>
       </c>
       <c r="L6" t="s">
         <v>75</v>
       </c>
       <c r="M6">
-        <v>24.924</v>
+        <v>0.368</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="O6">
-        <v>34.555</v>
+        <v>0.754</v>
       </c>
       <c r="P6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Q6">
-        <v>57.071</v>
+        <v>1.008</v>
       </c>
       <c r="R6" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="S6">
-        <v>21.191</v>
+        <v>0.331</v>
       </c>
       <c r="T6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="U6">
-        <v>32.576</v>
+        <v>0.977</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1142,61 +1409,61 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>24.27</v>
+        <v>0.268</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
       </c>
       <c r="E7">
-        <v>41.157</v>
+        <v>0.915</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7">
-        <v>51.026</v>
+        <v>1.43</v>
       </c>
       <c r="H7" t="s">
         <v>57</v>
       </c>
       <c r="I7">
-        <v>18.564</v>
+        <v>0.464</v>
       </c>
       <c r="J7" t="s">
         <v>66</v>
       </c>
       <c r="K7">
-        <v>9.044</v>
+        <v>0.204</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="M7">
-        <v>23.149</v>
+        <v>0.333</v>
       </c>
       <c r="N7" t="s">
         <v>83</v>
       </c>
       <c r="O7">
-        <v>34.434</v>
+        <v>0.75</v>
       </c>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q7">
-        <v>56.726</v>
+        <v>1.001</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="S7">
-        <v>18.251</v>
+        <v>0.171</v>
       </c>
       <c r="T7" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="U7">
-        <v>30.289</v>
+        <v>0.947</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1207,61 +1474,61 @@
         <v>26</v>
       </c>
       <c r="C8">
-        <v>23.894</v>
+        <v>0.262</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
       </c>
       <c r="E8">
-        <v>40.832</v>
+        <v>0.896</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8">
-        <v>43.838</v>
+        <v>1.253</v>
       </c>
       <c r="H8" t="s">
         <v>58</v>
       </c>
       <c r="I8">
-        <v>17.872</v>
+        <v>0.458</v>
       </c>
       <c r="J8" t="s">
         <v>67</v>
       </c>
       <c r="K8">
-        <v>9.026</v>
+        <v>0.195</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M8">
-        <v>21.823</v>
+        <v>0.318</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="O8">
-        <v>33.579</v>
+        <v>0.749</v>
       </c>
       <c r="P8" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="Q8">
-        <v>53.028</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="S8">
-        <v>16.461</v>
+        <v>0.162</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="U8">
-        <v>28.853</v>
+        <v>0.924</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1272,61 +1539,61 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>23.664</v>
+        <v>0.259</v>
       </c>
       <c r="D9" t="s">
         <v>38</v>
       </c>
       <c r="E9">
-        <v>39.989</v>
+        <v>0.876</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9">
-        <v>43.428</v>
+        <v>1.244</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I9">
-        <v>17.386</v>
+        <v>0.454</v>
       </c>
       <c r="J9" t="s">
         <v>68</v>
       </c>
       <c r="K9">
-        <v>8.946999999999999</v>
+        <v>0.187</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="M9">
-        <v>20.553</v>
+        <v>0.292</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="O9">
-        <v>30.678</v>
+        <v>0.611</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="Q9">
-        <v>51.368</v>
+        <v>0.857</v>
       </c>
       <c r="R9" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="S9">
-        <v>11.493</v>
+        <v>0.155</v>
       </c>
       <c r="T9" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="U9">
-        <v>26.676</v>
+        <v>0.846</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1337,61 +1604,61 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>22.528</v>
+        <v>0.251</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
       </c>
       <c r="E10">
-        <v>38.526</v>
+        <v>0.871</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G10">
-        <v>40.101</v>
+        <v>1.241</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10">
-        <v>16.862</v>
+        <v>0.379</v>
       </c>
       <c r="J10" t="s">
         <v>69</v>
       </c>
       <c r="K10">
-        <v>8.785</v>
+        <v>0.181</v>
       </c>
       <c r="L10" t="s">
         <v>78</v>
       </c>
       <c r="M10">
-        <v>20.306</v>
+        <v>0.289</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="O10">
-        <v>30.144</v>
+        <v>0.553</v>
       </c>
       <c r="P10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="Q10">
-        <v>51.207</v>
+        <v>0.855</v>
       </c>
       <c r="R10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="S10">
-        <v>10.483</v>
+        <v>0.148</v>
       </c>
       <c r="T10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="U10">
-        <v>23.964</v>
+        <v>0.715</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1402,61 +1669,61 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>22.518</v>
+        <v>0.248</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
       </c>
       <c r="E11">
-        <v>38.112</v>
+        <v>0.87</v>
       </c>
       <c r="F11" t="s">
         <v>50</v>
       </c>
       <c r="G11">
-        <v>39.948</v>
+        <v>1.221</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11">
-        <v>15.137</v>
+        <v>0.369</v>
       </c>
       <c r="J11" t="s">
         <v>70</v>
       </c>
       <c r="K11">
-        <v>8.677</v>
+        <v>0.144</v>
       </c>
       <c r="L11" t="s">
         <v>79</v>
       </c>
       <c r="M11">
-        <v>19.774</v>
+        <v>0.257</v>
       </c>
       <c r="N11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="O11">
-        <v>29.562</v>
+        <v>0.542</v>
       </c>
       <c r="P11" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="Q11">
-        <v>49.922</v>
+        <v>0.84</v>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="S11">
-        <v>6.972</v>
+        <v>0.122</v>
       </c>
       <c r="T11" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="U11">
-        <v>23.045</v>
+        <v>0.706</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1467,61 +1734,61 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>21.621</v>
+        <v>0.246</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E12">
-        <v>38.111</v>
+        <v>0.869</v>
       </c>
       <c r="F12" t="s">
         <v>51</v>
       </c>
       <c r="G12">
-        <v>35.947</v>
+        <v>1.196</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12">
-        <v>15.073</v>
+        <v>0.283</v>
       </c>
       <c r="J12" t="s">
         <v>71</v>
       </c>
       <c r="K12">
-        <v>8.393000000000001</v>
+        <v>0.131</v>
       </c>
       <c r="L12" t="s">
         <v>80</v>
       </c>
       <c r="M12">
-        <v>18.91</v>
+        <v>0.252</v>
       </c>
       <c r="N12" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="O12">
-        <v>28.806</v>
+        <v>0.463</v>
       </c>
       <c r="P12" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="Q12">
-        <v>49.552</v>
+        <v>0.838</v>
       </c>
       <c r="R12" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="S12">
-        <v>6.873</v>
+        <v>0.116</v>
       </c>
       <c r="T12" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="U12">
-        <v>22.919</v>
+        <v>0.647</v>
       </c>
     </row>
   </sheetData>
@@ -1616,7 +1883,7 @@
         <v>0.003</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>10.456</v>
@@ -1628,7 +1895,7 @@
         <v>28.391</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <v>78.13</v>
@@ -1646,19 +1913,19 @@
         <v>32.6</v>
       </c>
       <c r="P2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q2">
         <v>4.952</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S2">
         <v>32.507</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="U2">
         <v>32.864</v>
@@ -1672,61 +1939,61 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>173.47</v>
+        <v>2.281</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="E3">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>43</v>
       </c>
       <c r="G3">
-        <v>8.983000000000001</v>
+        <v>0.073</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="I3">
-        <v>16.092</v>
+        <v>0.257</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="K3">
-        <v>48.235</v>
+        <v>1.262</v>
       </c>
       <c r="L3" t="s">
         <v>73</v>
       </c>
       <c r="M3">
-        <v>39.054</v>
+        <v>0.524</v>
       </c>
       <c r="N3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O3">
-        <v>28.752</v>
+        <v>0.412</v>
       </c>
       <c r="P3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="Q3">
-        <v>7.644</v>
+        <v>0.065</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="S3">
-        <v>18.713</v>
+        <v>0.345</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="U3">
-        <v>29.535</v>
+        <v>0.285</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1734,64 +2001,64 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>128.488</v>
+        <v>1.278</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="E4">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G4">
-        <v>8.845000000000001</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="I4">
-        <v>14.827</v>
+        <v>0.181</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="K4">
-        <v>43.807</v>
+        <v>1.142</v>
       </c>
       <c r="L4" t="s">
         <v>74</v>
       </c>
       <c r="M4">
-        <v>38.391</v>
+        <v>0.404</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="O4">
-        <v>27.049</v>
+        <v>0.395</v>
       </c>
       <c r="P4" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="Q4">
-        <v>6.205</v>
+        <v>0.043</v>
       </c>
       <c r="R4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="S4">
-        <v>18.304</v>
+        <v>0.304</v>
       </c>
       <c r="T4" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
       <c r="U4">
-        <v>23.872</v>
+        <v>0.274</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1799,64 +2066,64 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="C5">
-        <v>125.222</v>
+        <v>1.247</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="E5">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5">
-        <v>7.455</v>
+        <v>0.064</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="I5">
-        <v>14.274</v>
+        <v>0.172</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
       <c r="K5">
-        <v>41.885</v>
+        <v>1.135</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M5">
-        <v>37.928</v>
+        <v>0.374</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="O5">
-        <v>26.058</v>
+        <v>0.301</v>
       </c>
       <c r="P5" t="s">
         <v>47</v>
       </c>
       <c r="Q5">
-        <v>6.172</v>
+        <v>0.041</v>
       </c>
       <c r="R5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="S5">
-        <v>17.869</v>
+        <v>0.264</v>
       </c>
       <c r="T5" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="U5">
-        <v>22.148</v>
+        <v>0.273</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1864,64 +2131,64 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>112.577</v>
+        <v>1.167</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="E6">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G6">
-        <v>7.336</v>
+        <v>0.063</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="I6">
-        <v>14.171</v>
+        <v>0.162</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="K6">
-        <v>41.505</v>
+        <v>1.115</v>
       </c>
       <c r="L6" t="s">
         <v>75</v>
       </c>
       <c r="M6">
-        <v>34.224</v>
+        <v>0.364</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="O6">
-        <v>25.18</v>
+        <v>0.283</v>
       </c>
       <c r="P6" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="Q6">
-        <v>5.479</v>
+        <v>0.039</v>
       </c>
       <c r="R6" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="S6">
-        <v>16.486</v>
+        <v>0.097</v>
       </c>
       <c r="T6" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="U6">
-        <v>21.741</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1929,64 +2196,64 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>108.879</v>
+        <v>1.107</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="E7">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G7">
-        <v>6.879</v>
+        <v>0.058</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="I7">
-        <v>13.696</v>
+        <v>0.151</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="K7">
-        <v>40.853</v>
+        <v>1.103</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="M7">
-        <v>31.786</v>
+        <v>0.347</v>
       </c>
       <c r="N7" t="s">
-        <v>83</v>
+        <v>155</v>
       </c>
       <c r="O7">
-        <v>25.092</v>
+        <v>0.267</v>
       </c>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="Q7">
-        <v>5.445</v>
+        <v>0.037</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="S7">
-        <v>14.199</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="T7" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
       <c r="U7">
-        <v>20.214</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1994,64 +2261,64 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C8">
-        <v>107.196</v>
+        <v>1.083</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="E8">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="G8">
-        <v>5.91</v>
+        <v>0.057</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="I8">
-        <v>13.185</v>
+        <v>0.15</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="K8">
-        <v>40.77</v>
+        <v>1.074</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M8">
-        <v>29.966</v>
+        <v>0.33</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="O8">
-        <v>24.469</v>
+        <v>0.248</v>
       </c>
       <c r="P8" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="Q8">
-        <v>5.09</v>
+        <v>0.037</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="S8">
-        <v>12.807</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="U8">
-        <v>19.256</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -2059,64 +2326,64 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="C9">
-        <v>106.163</v>
+        <v>1.08</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="E9">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="G9">
-        <v>5.855</v>
+        <v>0.056</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="I9">
-        <v>12.827</v>
+        <v>0.15</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="K9">
-        <v>40.416</v>
+        <v>1.073</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="M9">
-        <v>28.221</v>
+        <v>0.306</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="O9">
-        <v>22.355</v>
+        <v>0.242</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="Q9">
-        <v>4.931</v>
+        <v>0.035</v>
       </c>
       <c r="R9" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="S9">
-        <v>8.941000000000001</v>
+        <v>0.067</v>
       </c>
       <c r="T9" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="U9">
-        <v>17.803</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2127,61 +2394,61 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>101.068</v>
+        <v>1.07</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="E10">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G10">
-        <v>5.406</v>
+        <v>0.053</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="I10">
-        <v>12.44</v>
+        <v>0.135</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="K10">
-        <v>39.681</v>
+        <v>1.053</v>
       </c>
       <c r="L10" t="s">
         <v>78</v>
       </c>
       <c r="M10">
-        <v>27.883</v>
+        <v>0.301</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="O10">
-        <v>21.966</v>
+        <v>0.234</v>
       </c>
       <c r="P10" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="Q10">
-        <v>4.916</v>
+        <v>0.033</v>
       </c>
       <c r="R10" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
       <c r="S10">
-        <v>8.154999999999999</v>
+        <v>0.063</v>
       </c>
       <c r="T10" t="s">
-        <v>110</v>
+        <v>174</v>
       </c>
       <c r="U10">
-        <v>15.993</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -2192,61 +2459,61 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>101.022</v>
+        <v>1.061</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="E11">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="G11">
-        <v>5.386</v>
+        <v>0.045</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="I11">
-        <v>11.167</v>
+        <v>0.076</v>
       </c>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="K11">
-        <v>39.195</v>
+        <v>1.008</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="M11">
-        <v>27.152</v>
+        <v>0.279</v>
       </c>
       <c r="N11" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="O11">
-        <v>21.542</v>
+        <v>0.214</v>
       </c>
       <c r="P11" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="Q11">
-        <v>4.792</v>
+        <v>0.033</v>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
       <c r="S11">
-        <v>5.424</v>
+        <v>0.061</v>
       </c>
       <c r="T11" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="U11">
-        <v>15.38</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -2254,64 +2521,64 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="C12">
-        <v>96.998</v>
+        <v>1.055</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="E12">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <v>0.044</v>
+      </c>
+      <c r="H12" t="s">
+        <v>142</v>
+      </c>
+      <c r="I12">
+        <v>0.064</v>
+      </c>
+      <c r="J12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K12">
+        <v>0.92</v>
+      </c>
+      <c r="L12" t="s">
+        <v>152</v>
+      </c>
+      <c r="M12">
+        <v>0.278</v>
+      </c>
+      <c r="N12" t="s">
         <v>51</v>
       </c>
-      <c r="G12">
-        <v>4.846</v>
-      </c>
-      <c r="H12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12">
-        <v>11.12</v>
-      </c>
-      <c r="J12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12">
-        <v>37.911</v>
-      </c>
-      <c r="L12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12">
-        <v>25.966</v>
-      </c>
-      <c r="N12" t="s">
-        <v>85</v>
-      </c>
       <c r="O12">
-        <v>20.991</v>
+        <v>0.211</v>
       </c>
       <c r="P12" t="s">
-        <v>93</v>
+        <v>164</v>
       </c>
       <c r="Q12">
-        <v>4.757</v>
+        <v>0.032</v>
       </c>
       <c r="R12" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="S12">
-        <v>5.347</v>
+        <v>0.06</v>
       </c>
       <c r="T12" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="U12">
-        <v>15.296</v>
+        <v>0.146</v>
       </c>
     </row>
   </sheetData>
@@ -2406,7 +2673,7 @@
         <v>11.083</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>24.769</v>
@@ -2418,7 +2685,7 @@
         <v>5.908</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <v>60.309</v>
@@ -2436,19 +2703,19 @@
         <v>4.188</v>
       </c>
       <c r="P2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q2">
         <v>31.663</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S2">
         <v>91.64100000000001</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="U2">
         <v>52.77</v>
@@ -2462,61 +2729,61 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>167.911</v>
+        <v>2.223</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3">
-        <v>7.682</v>
+        <v>0.096</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G3">
-        <v>21.281</v>
+        <v>0.204</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="I3">
-        <v>3.349</v>
+        <v>0.036</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="K3">
-        <v>37.233</v>
+        <v>0.586</v>
       </c>
       <c r="L3" t="s">
         <v>73</v>
       </c>
       <c r="M3">
-        <v>41.633</v>
+        <v>1.047</v>
       </c>
       <c r="N3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O3">
-        <v>3.693</v>
+        <v>0.04</v>
       </c>
       <c r="P3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="Q3">
-        <v>48.874</v>
+        <v>0.495</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="S3">
-        <v>52.756</v>
+        <v>4.343</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="U3">
-        <v>47.426</v>
+        <v>0.403</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2524,64 +2791,64 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>124.37</v>
+        <v>1.274</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4">
-        <v>7.575</v>
+        <v>0.089</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="G4">
-        <v>20.952</v>
+        <v>0.182</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="I4">
-        <v>3.086</v>
+        <v>0.027</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>190</v>
       </c>
       <c r="K4">
-        <v>33.815</v>
+        <v>0.522</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M4">
-        <v>40.926</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="O4">
-        <v>3.474</v>
+        <v>0.038</v>
       </c>
       <c r="P4" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="Q4">
-        <v>39.673</v>
+        <v>0.334</v>
       </c>
       <c r="R4" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="S4">
-        <v>51.601</v>
+        <v>3.129</v>
       </c>
       <c r="T4" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
       <c r="U4">
-        <v>38.331</v>
+        <v>0.388</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -2589,64 +2856,64 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5">
-        <v>121.209</v>
+        <v>1.104</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
       </c>
       <c r="E5">
-        <v>7.4</v>
+        <v>0.089</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>182</v>
       </c>
       <c r="G5">
-        <v>17.66</v>
+        <v>0.181</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="I5">
-        <v>2.971</v>
+        <v>0.025</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="K5">
-        <v>32.331</v>
+        <v>0.44</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="M5">
-        <v>40.432</v>
+        <v>0.725</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="O5">
-        <v>3.347</v>
+        <v>0.029</v>
       </c>
       <c r="P5" t="s">
         <v>47</v>
       </c>
       <c r="Q5">
-        <v>39.463</v>
+        <v>0.304</v>
       </c>
       <c r="R5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S5">
-        <v>50.375</v>
+        <v>2.084</v>
       </c>
       <c r="T5" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="U5">
-        <v>35.563</v>
+        <v>0.386</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -2654,64 +2921,64 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>108.97</v>
+        <v>1.092</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
       </c>
       <c r="E6">
-        <v>7.344</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="G6">
-        <v>17.378</v>
+        <v>0.179</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="I6">
-        <v>2.949</v>
+        <v>0.023</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="K6">
-        <v>32.038</v>
+        <v>0.428</v>
       </c>
       <c r="L6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M6">
-        <v>36.483</v>
+        <v>0.703</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="O6">
-        <v>3.234</v>
+        <v>0.027</v>
       </c>
       <c r="P6" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="Q6">
-        <v>35.031</v>
+        <v>0.287</v>
       </c>
       <c r="R6" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="S6">
-        <v>46.477</v>
+        <v>1.817</v>
       </c>
       <c r="T6" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="U6">
-        <v>34.909</v>
+        <v>0.349</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -2719,64 +2986,64 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>105.39</v>
+        <v>1.062</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7">
-        <v>7.244</v>
+        <v>0.08</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>184</v>
       </c>
       <c r="G7">
-        <v>16.296</v>
+        <v>0.171</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="I7">
-        <v>2.85</v>
+        <v>0.022</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="K7">
-        <v>31.534</v>
+        <v>0.405</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="M7">
-        <v>33.885</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="N7" t="s">
-        <v>83</v>
+        <v>155</v>
       </c>
       <c r="O7">
-        <v>3.223</v>
+        <v>0.026</v>
       </c>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="Q7">
-        <v>34.819</v>
+        <v>0.268</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S7">
-        <v>40.029</v>
+        <v>1.588</v>
       </c>
       <c r="T7" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
       <c r="U7">
-        <v>32.458</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2784,64 +3051,64 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="C8">
-        <v>103.761</v>
+        <v>1.046</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>177</v>
       </c>
       <c r="E8">
-        <v>7.187</v>
+        <v>0.076</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>185</v>
       </c>
       <c r="G8">
-        <v>14</v>
+        <v>0.166</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="I8">
-        <v>2.744</v>
+        <v>0.022</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="K8">
-        <v>31.471</v>
+        <v>0.385</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="M8">
-        <v>31.944</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="O8">
-        <v>3.143</v>
+        <v>0.024</v>
       </c>
       <c r="P8" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="Q8">
-        <v>32.549</v>
+        <v>0.267</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="S8">
-        <v>36.104</v>
+        <v>0.909</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="U8">
-        <v>30.92</v>
+        <v>0.299</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -2849,64 +3116,64 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C9">
-        <v>102.761</v>
+        <v>1.044</v>
       </c>
       <c r="D9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9">
+        <v>0.075</v>
+      </c>
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9">
+        <v>0.159</v>
+      </c>
+      <c r="H9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9">
+        <v>0.021</v>
+      </c>
+      <c r="J9" t="s">
         <v>38</v>
       </c>
-      <c r="E9">
-        <v>7.039</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9">
-        <v>13.869</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9">
-        <v>2.669</v>
-      </c>
-      <c r="J9" t="s">
-        <v>68</v>
-      </c>
       <c r="K9">
-        <v>31.198</v>
+        <v>0.381</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
       <c r="M9">
-        <v>30.085</v>
+        <v>0.541</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="O9">
-        <v>2.872</v>
+        <v>0.024</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="Q9">
-        <v>31.53</v>
+        <v>0.25</v>
       </c>
       <c r="R9" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="S9">
-        <v>25.207</v>
+        <v>0.886</v>
       </c>
       <c r="T9" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="U9">
-        <v>28.587</v>
+        <v>0.287</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2914,64 +3181,64 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10">
-        <v>97.82899999999999</v>
+        <v>1.041</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>179</v>
       </c>
       <c r="E10">
-        <v>6.781</v>
+        <v>0.074</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="G10">
-        <v>12.807</v>
+        <v>0.131</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="I10">
-        <v>2.589</v>
+        <v>0.019</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="K10">
-        <v>30.63</v>
+        <v>0.378</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M10">
-        <v>29.724</v>
+        <v>0.498</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="O10">
-        <v>2.821</v>
+        <v>0.023</v>
       </c>
       <c r="P10" t="s">
-        <v>92</v>
+        <v>163</v>
       </c>
       <c r="Q10">
-        <v>31.431</v>
+        <v>0.249</v>
       </c>
       <c r="R10" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="S10">
-        <v>22.991</v>
+        <v>0.87</v>
       </c>
       <c r="T10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="U10">
-        <v>25.681</v>
+        <v>0.267</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -2979,64 +3246,64 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="C11">
-        <v>97.785</v>
+        <v>1.02</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
       </c>
       <c r="E11">
-        <v>6.708</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="G11">
-        <v>12.758</v>
+        <v>0.127</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="I11">
-        <v>2.324</v>
+        <v>0.011</v>
       </c>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="K11">
-        <v>30.255</v>
+        <v>0.371</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>192</v>
       </c>
       <c r="M11">
-        <v>28.945</v>
+        <v>0.461</v>
       </c>
       <c r="N11" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="O11">
-        <v>2.767</v>
+        <v>0.021</v>
       </c>
       <c r="P11" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="Q11">
-        <v>30.643</v>
+        <v>0.242</v>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="S11">
-        <v>15.291</v>
+        <v>0.712</v>
       </c>
       <c r="T11" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="U11">
-        <v>24.696</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -3044,64 +3311,64 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12">
-        <v>93.89</v>
+        <v>0.987</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="E12">
-        <v>6.708</v>
+        <v>0.066</v>
       </c>
       <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>0.118</v>
+      </c>
+      <c r="H12" t="s">
+        <v>142</v>
+      </c>
+      <c r="I12">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="J12" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12">
+        <v>0.367</v>
+      </c>
+      <c r="L12" t="s">
+        <v>193</v>
+      </c>
+      <c r="M12">
+        <v>0.436</v>
+      </c>
+      <c r="N12" t="s">
         <v>51</v>
       </c>
-      <c r="G12">
-        <v>11.48</v>
-      </c>
-      <c r="H12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12">
-        <v>2.314</v>
-      </c>
-      <c r="J12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12">
-        <v>29.264</v>
-      </c>
-      <c r="L12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12">
-        <v>27.68</v>
-      </c>
-      <c r="N12" t="s">
-        <v>85</v>
-      </c>
       <c r="O12">
-        <v>2.696</v>
+        <v>0.02</v>
       </c>
       <c r="P12" t="s">
-        <v>93</v>
+        <v>195</v>
       </c>
       <c r="Q12">
-        <v>30.415</v>
+        <v>0.236</v>
       </c>
       <c r="R12" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="S12">
-        <v>15.073</v>
+        <v>0.661</v>
       </c>
       <c r="T12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U12">
-        <v>24.561</v>
+        <v>0.261</v>
       </c>
     </row>
   </sheetData>
@@ -3196,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3208,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3226,19 +3493,19 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3249,61 +3516,61 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3314,61 +3581,61 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -3379,61 +3646,61 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -3444,61 +3711,61 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -3509,61 +3776,61 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -3574,61 +3841,61 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -3639,61 +3906,61 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -3704,61 +3971,61 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -3769,61 +4036,61 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -3834,61 +4101,61 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -3986,7 +4253,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3998,7 +4265,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4016,19 +4283,19 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4039,61 +4306,61 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4104,61 +4371,61 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>114</v>
+        <v>203</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -4169,61 +4436,61 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -4234,61 +4501,61 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -4299,61 +4566,61 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -4364,61 +4631,61 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -4429,61 +4696,61 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -4494,61 +4761,61 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -4559,61 +4826,61 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -4624,61 +4891,61 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="U12">
         <v>0</v>

</xml_diff>